<commit_message>
El error del vacio persiste
</commit_message>
<xml_diff>
--- a/Historial de Comits/Historial de Comits.xlsx
+++ b/Historial de Comits/Historial de Comits.xlsx
@@ -2,14 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Octavio\Desktop\I.R.O.J.I\Historial de Comits\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -18,12 +23,52 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+  <si>
+    <t xml:space="preserve">Fecha </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrante </t>
+  </si>
+  <si>
+    <t>Titulo del Comit</t>
+  </si>
+  <si>
+    <t>Descripcion del Comit</t>
+  </si>
+  <si>
+    <t>Brumer arregla bug al vacio Apollyon Triste</t>
+  </si>
+  <si>
+    <t>Se arregla el error en el que 2 salas chocan y generan un vacio</t>
+  </si>
+  <si>
+    <t>Octavio Lucardi Fierro</t>
+  </si>
+  <si>
+    <t>El error del vacio persiste</t>
+  </si>
+  <si>
+    <t>Al actualizar el repositorio y correr el codigo, este ya no reconoce la librería de Unity y deja de funcionar todo</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -46,13 +91,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -331,12 +390,174 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" customWidth="1"/>
+    <col min="4" max="4" width="52.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>44721</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>44721</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" display="https://github.com/ipopotamo/I.R.O.J.I/commit/20f1e72b5ff7299972145393c3bbdd169b4b2609"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Juan camina y gira
</commit_message>
<xml_diff>
--- a/Historial de Comits/Historial de Comits.xlsx
+++ b/Historial de Comits/Historial de Comits.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t xml:space="preserve">Fecha </t>
   </si>
@@ -62,13 +62,19 @@
     <t>Juan cuenta con una barra de vida funcional</t>
   </si>
   <si>
-    <t>Juan ya tiene una barra de vida arriba a la izquierda, y se creo un fuego para que este pierda 10% de su vida y muera</t>
-  </si>
-  <si>
     <t>Juan recupera vida</t>
   </si>
   <si>
     <t>Juan recupera vida un 50 % de vida con un item de dudosa procedencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juan camina y gira </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juan hace una animacion al caminar y gira en direccion al mouse </t>
+  </si>
+  <si>
+    <t>Juan ya tiene una barra de vida arriba a la izquierda, y se creo un fuego para que este pierda 10% de su vida y muera y una sorpresa al suceder esto.</t>
   </si>
 </sst>
 </file>
@@ -438,7 +444,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,7 +527,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -532,18 +538,26 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>44724</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="D8" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>

</xml_diff>

<commit_message>
Juan camina bien + menu de opciones
</commit_message>
<xml_diff>
--- a/Historial de Comits/Historial de Comits.xlsx
+++ b/Historial de Comits/Historial de Comits.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t xml:space="preserve">Fecha </t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>Juan ya tiene una barra de vida arriba a la izquierda, y se creo un fuego para que este pierda 10% de su vida y muera y una sorpresa al suceder esto.</t>
+  </si>
+  <si>
+    <t>Juan camina bien + menu de opciones</t>
+  </si>
+  <si>
+    <t>Juan tiene bien hechas las animaciones, hay un menu de opciones que regula el sonido y la pantalla completa y se intenta disparar</t>
   </si>
 </sst>
 </file>
@@ -142,7 +148,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -160,6 +166,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -444,7 +456,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,11 +571,19 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>44727</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>

</xml_diff>

<commit_message>
RIOOOOOOOOOS necesito los enemigos, asi que jodete momentaneamente
</commit_message>
<xml_diff>
--- a/Historial de Comits/Historial de Comits.xlsx
+++ b/Historial de Comits/Historial de Comits.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t xml:space="preserve">Fecha </t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>Juan tiene bien hechas las animaciones, hay un menu de opciones que regula el sonido y la pantalla completa y se intenta disparar</t>
+  </si>
+  <si>
+    <t>Juan no tiene esqueleto para hacer animaciones, pero pega un pequeño golpe hacia adelante, Se añade el primer intento de enemigo</t>
+  </si>
+  <si>
+    <t>RIOOOOOOOOOS necesito los enemigos, asi que jodete momentaneamente</t>
   </si>
 </sst>
 </file>
@@ -456,7 +462,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,11 +591,19 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>44737</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>

</xml_diff>

<commit_message>
CHICOS AYUDAAAA QUE ALGUIEN MAS HAGA SPRITES PORQUE ES HORRIBLE
</commit_message>
<xml_diff>
--- a/Historial de Comits/Historial de Comits.xlsx
+++ b/Historial de Comits/Historial de Comits.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t xml:space="preserve">Fecha </t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>RIOOOOOOOOOS necesito los enemigos, asi que jodete momentaneamente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHICOS AYUDAAAA QUE ALGUIEN MAS HAGA SPRITES PORQUE ES HORRIBLE </t>
+  </si>
+  <si>
+    <t>juan tien 2 tipos de ataque, un apuñalamiento a poca distancia y otro como un barrido, al cual no le funciona la animacion porque UNITY no me deja hacer la cosas igual que en los tutoriales</t>
   </si>
 </sst>
 </file>
@@ -462,7 +468,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,11 +611,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>44737</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>

</xml_diff>